<commit_message>
Update the report templates
</commit_message>
<xml_diff>
--- a/resource/TEMPLATE_china_stock_tradings.xlsx
+++ b/resource/TEMPLATE_china_stock_tradings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\COCOA\Hole\ARK\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\COCOA\Hole\ARK\Resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7EB6DE-0AD0-4A9A-9794-31356AE2AB6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12798BC8-B1C4-4541-9C7C-5D6F3191F930}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="1440" windowWidth="21015" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +80,13 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei UI Light"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="4">
@@ -114,7 +121,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -126,6 +133,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -411,7 +421,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -437,158 +447,158 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
@@ -669,6 +679,7 @@
     <row r="40" spans="1:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>